<commit_message>
Update error suite table
</commit_message>
<xml_diff>
--- a/error_suite/exceptions.xlsx
+++ b/error_suite/exceptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tWX1238545\IdeaProjects\UTBotPythonSamples\error_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45EF6722-5E00-4D9B-A982-E9E719CAF589}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE201ED3-0F37-42FF-B560-24EF72D4424E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18450" windowHeight="11348" xr2:uid="{512A67AE-FE94-4820-8E80-29EC1421240B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$C$1:$C$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$D$1:$D$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t>caldav</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>pylint</t>
+  </si>
+  <si>
+    <t>https://github.com/python-caldav/caldav</t>
+  </si>
+  <si>
+    <t>https://github.com/TheAlgorithms/Python</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/tamarinvs19/misterX/</t>
+  </si>
+  <si>
+    <t>https://github.com/pylint-dev/pylint/</t>
   </si>
 </sst>
 </file>
@@ -624,539 +636,551 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5E96C4-809E-41CC-9767-FB1C50EFFB5B}">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="63.53125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" customWidth="1"/>
+    <col min="3" max="3" width="63.53125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="3" t="s">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="4" t="s">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="4" t="s">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="4" t="s">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="4" t="s">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="4" t="s">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="4" t="s">
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="4" t="s">
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="4" t="s">
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="4" t="s">
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="4" t="s">
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="4" t="s">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" s="4" t="s">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B28" s="4" t="s">
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B29" s="4" t="s">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B30" s="4" t="s">
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B31" s="4" t="s">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B32" s="4" t="s">
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" s="4" t="s">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B35" s="4" t="s">
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B36" s="4" t="s">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B37" s="4" t="s">
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B38" s="4" t="s">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B39" s="4" t="s">
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B40" s="4" t="s">
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C40" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B41" s="4" t="s">
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C41" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B42" s="4" t="s">
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B43" s="4" t="s">
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B44" s="4" t="s">
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B45" s="4" t="s">
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C45" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B46" s="4" t="s">
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B47" s="4" t="s">
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B48" s="4" t="s">
+      <c r="D47" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C48" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B49" s="4" t="s">
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C49" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B50" s="4" t="s">
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C50" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B51" s="4" t="s">
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C51" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B52" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B53" s="4" t="s">
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C53" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B54" s="4" t="s">
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B55" s="4" t="s">
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C55" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B56" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B57" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C57" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B58" s="4" t="s">
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C58" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B59" s="4" t="s">
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C59" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B60" s="4" t="s">
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C60" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B61" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C61" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B70" s="1"/>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C70" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C63" xr:uid="{2741DD63-9340-4D4E-8FFC-E0A1A271B609}"/>
+  <autoFilter ref="D1:D63" xr:uid="{2741DD63-9340-4D4E-8FFC-E0A1A271B609}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>